<commit_message>
added fetch subjects data
</commit_message>
<xml_diff>
--- a/public/upload_data_files/student_format.xlsx
+++ b/public/upload_data_files/student_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham\learning\BPIT\Attendance\bpit_admin_panel\public\upload_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DFAA0E-2DCC-4DC5-AFB3-9AE6BEDDC8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63758085-E2F5-4BF7-887A-AB3861425481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>enrollment_number</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>A,B,C (IF THERE IS ONLY ONE SECTION ADD "A")</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>1,2,3 (depending on MBA,BBA,Btech respectively)</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,19 +449,20 @@
     <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,34 +473,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -504,37 +514,40 @@
         <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{1985BF32-29A3-4839-A193-A7EC5C9CEC53}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{1985BF32-29A3-4839-A193-A7EC5C9CEC53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added fetch subjects data (#17)
</commit_message>
<xml_diff>
--- a/public/upload_data_files/student_format.xlsx
+++ b/public/upload_data_files/student_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shubham\learning\BPIT\Attendance\bpit_admin_panel\public\upload_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DFAA0E-2DCC-4DC5-AFB3-9AE6BEDDC8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63758085-E2F5-4BF7-887A-AB3861425481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>enrollment_number</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>A,B,C (IF THERE IS ONLY ONE SECTION ADD "A")</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>1,2,3 (depending on MBA,BBA,Btech respectively)</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,19 +449,20 @@
     <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,34 +473,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -504,37 +514,40 @@
         <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{1985BF32-29A3-4839-A193-A7EC5C9CEC53}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{1985BF32-29A3-4839-A193-A7EC5C9CEC53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>